<commit_message>
push data to excel
</commit_message>
<xml_diff>
--- a/Data1.xlsx
+++ b/Data1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/859bc52c1c1b6f5c/Documents/GitHub/SEFinal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junyuyao/Documents/GitHub/SEFinal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{982301D6-2010-2945-B8C6-5365A1C0ED80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{442E994E-A459-45BF-BC55-77B8F42F32AF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE1BFCA-F4C3-5441-AECF-62CDF3B5E185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2740" yWindow="2740" windowWidth="26760" windowHeight="11380" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="League" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="Sport" sheetId="3" r:id="rId3"/>
     <sheet name="Organizer" sheetId="4" r:id="rId4"/>
     <sheet name="Team" sheetId="5" r:id="rId5"/>
-    <sheet name="ViewTeams" sheetId="9" r:id="rId6"/>
-    <sheet name="ViewLeagueName" sheetId="11" r:id="rId7"/>
-    <sheet name="ViewStandings" sheetId="10" r:id="rId8"/>
-    <sheet name="Referee" sheetId="6" r:id="rId9"/>
-    <sheet name="Player" sheetId="7" r:id="rId10"/>
-    <sheet name="Highlight" sheetId="8" r:id="rId11"/>
+    <sheet name="ViewTeams" sheetId="6" r:id="rId6"/>
+    <sheet name="ViewLeagueName" sheetId="7" r:id="rId7"/>
+    <sheet name="ViewStandings" sheetId="8" r:id="rId8"/>
+    <sheet name="Referee" sheetId="9" r:id="rId9"/>
+    <sheet name="Player" sheetId="10" r:id="rId10"/>
+    <sheet name="Highlight" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,6 +58,9 @@
     <t>Games</t>
   </si>
   <si>
+    <t>WAC Sports</t>
+  </si>
+  <si>
     <t>Game_ID</t>
   </si>
   <si>
@@ -106,18 +109,81 @@
     <t>Org_Name</t>
   </si>
   <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
     <t>Timmm</t>
   </si>
   <si>
+    <t>Smitty101</t>
+  </si>
+  <si>
+    <t>123456A</t>
+  </si>
+  <si>
     <t>Team_ID</t>
   </si>
   <si>
     <t>Team_Name</t>
   </si>
   <si>
+    <t>Player_Count</t>
+  </si>
+  <si>
+    <t>Jamisons</t>
+  </si>
+  <si>
+    <t>Jamies</t>
+  </si>
+  <si>
+    <t>Leos</t>
+  </si>
+  <si>
+    <t>Team Name</t>
+  </si>
+  <si>
+    <t>Player Count</t>
+  </si>
+  <si>
+    <t>TeamName</t>
+  </si>
+  <si>
+    <t>TeamCode</t>
+  </si>
+  <si>
+    <t>JMU Sports</t>
+  </si>
+  <si>
+    <t>ABC League</t>
+  </si>
+  <si>
+    <t>I hate Sports</t>
+  </si>
+  <si>
+    <t>Teams</t>
+  </si>
+  <si>
+    <t>Wins</t>
+  </si>
+  <si>
+    <t>Losses</t>
+  </si>
+  <si>
+    <t>Ties</t>
+  </si>
+  <si>
+    <t>Margs</t>
+  </si>
+  <si>
     <t>Ref_Name</t>
   </si>
   <si>
+    <t>Uersname</t>
+  </si>
+  <si>
     <t>Player_ID</t>
   </si>
   <si>
@@ -131,72 +197,6 @@
   </si>
   <si>
     <t>Player_Gender</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Uersname</t>
-  </si>
-  <si>
-    <t>Smitty101</t>
-  </si>
-  <si>
-    <t>123456A</t>
-  </si>
-  <si>
-    <t>Jamisons</t>
-  </si>
-  <si>
-    <t>Jamies</t>
-  </si>
-  <si>
-    <t>Leos</t>
-  </si>
-  <si>
-    <t>Player_Count</t>
-  </si>
-  <si>
-    <t>Player Count</t>
-  </si>
-  <si>
-    <t>Team Name</t>
-  </si>
-  <si>
-    <t>Teams</t>
-  </si>
-  <si>
-    <t>Wins</t>
-  </si>
-  <si>
-    <t>Losses</t>
-  </si>
-  <si>
-    <t>Ties</t>
-  </si>
-  <si>
-    <t>Margs</t>
-  </si>
-  <si>
-    <t>WAC Sports</t>
-  </si>
-  <si>
-    <t>TeamName</t>
-  </si>
-  <si>
-    <t>TeamCode</t>
-  </si>
-  <si>
-    <t>I hate Sports</t>
-  </si>
-  <si>
-    <t>ABC League</t>
-  </si>
-  <si>
-    <t>JMU Sports</t>
   </si>
 </sst>
 </file>
@@ -240,9 +240,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,9 +467,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,9 +486,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -497,7 +497,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -508,26 +508,26 @@
       <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -536,15 +536,17 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -559,32 +561,32 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -604,62 +606,62 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -678,34 +680,34 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -724,25 +726,25 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -751,9 +753,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -762,9 +764,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -779,28 +781,28 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE274071-4D5A-44F3-BAA5-0F322A9DA9FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="str">
         <f>Team!B2</f>
         <v>Jamisons</v>
@@ -810,7 +812,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="str">
         <f>Team!B3</f>
         <v>Jamies</v>
@@ -820,7 +822,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="str">
         <f>Team!B4</f>
         <v>Leos</v>
@@ -836,45 +838,45 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A23BAA-6B4E-425F-AEA9-15E00AFFDB8F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -886,32 +888,32 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D878CBF-391C-45AD-BD97-B3460739635C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -923,9 +925,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -937,9 +939,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -957,7 +959,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -967,20 +969,20 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>